<commit_message>
removed some not needed sightseeing
Signed-off-by: garumaru <harddies@126.com>
</commit_message>
<xml_diff>
--- a/sabah.xlsx
+++ b/sabah.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="行程" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF0070C0"/>
+        <color indexed="30"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -64,11 +64,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
+        <color indexed="30"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>红树林双配套优惠价马币</t>
     </r>
@@ -76,7 +74,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF0070C0"/>
+        <color indexed="30"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -86,11 +84,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
+        <color indexed="30"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>人</t>
     </r>
@@ -133,10 +129,8 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>开放时间：9:30~14:30 (平台A)，11:30~16:30（平台B）</t>
     </r>
@@ -144,10 +138,9 @@
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color indexed="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
 http://www.proboscis.cc</t>
@@ -269,10 +262,9 @@
         <b/>
         <u/>
         <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color indexed="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
       </rPr>
       <t>www.novotel.com/asia</t>
     </r>
@@ -285,10 +277,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
       </rPr>
       <t>网站</t>
     </r>
@@ -296,7 +287,7 @@
       <rPr>
         <b/>
         <sz val="10.5"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="新宋体"/>
         <family val="3"/>
         <charset val="134"/>
@@ -308,10 +299,9 @@
         <b/>
         <u/>
         <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
       </rPr>
       <t>www.thepalacehotelkk.com</t>
     </r>
@@ -328,26 +318,6 @@
   </si>
   <si>
     <t>环滩岛一日游</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dreamy Island Transport 梦之岛快艇DBKK 244530
- Kota Kinabalu, Sabah, Malaysia.
- +6016 803 3503(MR.Ang洪叔),
- +601119070966(Ms.Mun雅雯)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>环滩岛去不成。考虑迪加岛</t>
-    </r>
   </si>
   <si>
     <r>
@@ -364,10 +334,8 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>）红树林长鼻猴萤火虫一日游</t>
     </r>
@@ -377,83 +345,90 @@
   </si>
   <si>
     <t>海龟岛公园</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dreamy Island Transport 梦之岛快艇DBKK 244530
+ Kota Kinabalu, Sabah, Malaysia.
+ +6016 803 3503(MR.Ang洪叔),
+ +601119070966(Ms.Mun雅雯)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>环滩岛去不成。考虑迪加岛</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FF0070C0"/>
+      <color indexed="30"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <color indexed="36"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <color indexed="30"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <color indexed="30"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
+      <color indexed="30"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -463,77 +438,90 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color indexed="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <color indexed="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color indexed="8"/>
+      <name val="新宋体"/>
       <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10.5"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color indexed="36"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="新宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -546,7 +534,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,9 +602,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,20 +623,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,44 +641,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -708,31 +691,39 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>247163</xdr:colOff>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>94669</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2049" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4886325" y="209550"/>
-          <a:ext cx="3895238" cy="4647619"/>
+          <a:off x="5495925" y="190500"/>
+          <a:ext cx="4352925" cy="4191000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -746,31 +737,39 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304229</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>142238</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="2050" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="190500"/>
-          <a:ext cx="4571429" cy="5095238"/>
+          <a:off x="0" y="171450"/>
+          <a:ext cx="5105400" cy="4600575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -784,31 +783,39 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>580419</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>132860</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="2051" name="Picture 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9144000" y="209550"/>
-          <a:ext cx="4847619" cy="3923810"/>
+          <a:off x="10287000" y="190500"/>
+          <a:ext cx="5381625" cy="3543300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -822,31 +829,39 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>113753</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>46953</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="2052" name="Picture 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14630400" y="190500"/>
-          <a:ext cx="4380953" cy="5380953"/>
+          <a:off x="16459200" y="171450"/>
+          <a:ext cx="4914900" cy="4848225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -929,7 +944,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -964,7 +978,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1140,294 +1153,294 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" customWidth="1"/>
+    <col min="5" max="5" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="21">
+      <c r="A2" s="23">
         <v>41612</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="22"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="22"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="23"/>
-      <c r="B5" s="14">
+      <c r="A5" s="25"/>
+      <c r="B5" s="13">
         <v>0.92361111111111116</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="21">
+      <c r="A6" s="23">
         <v>41613</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="22"/>
-      <c r="B8" s="14">
+      <c r="A8" s="24"/>
+      <c r="B8" s="13">
         <v>0.625</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="23"/>
-      <c r="B9" s="14">
+      <c r="A9" s="25"/>
+      <c r="B9" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="24">
+      <c r="A10" s="19">
         <v>41614</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="25"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="25"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="24">
+      <c r="A13" s="19">
         <v>41615</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="25"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="25"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="24">
+      <c r="A16" s="19">
         <v>41616</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="25"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="25"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="24">
+      <c r="A19" s="19">
         <v>41617</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15" t="s">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="25"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1436,12 +1449,14 @@
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1449,28 +1464,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.75" customWidth="1"/>
+    <col min="3" max="3" width="33.875" customWidth="1"/>
+    <col min="4" max="4" width="72.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1493,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="94.5">
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="85.5">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1513,26 +1529,26 @@
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" s="21" customFormat="1" ht="67.5">
+      <c r="A6" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>56</v>
+      <c r="D6" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1">
-      <c r="A8" s="9" t="s">
-        <v>57</v>
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="14.25">
+      <c r="A8" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -1543,13 +1559,13 @@
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="45">
+    <row r="9" spans="1:5" s="4" customFormat="1" ht="40.5">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
@@ -1557,14 +1573,14 @@
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="20"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
@@ -1577,7 +1593,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1597,7 +1613,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1605,14 +1621,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1622,23 +1639,24 @@
       <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="17" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="http://www.grandborneohotel.com/"/>
     <hyperlink ref="I1" r:id="rId2" display="http://www.minggardenhotel.com/"/>
@@ -1650,7 +1668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
@@ -1658,14 +1676,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -1673,14 +1692,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>
@@ -1690,8 +1710,9 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Signed-off-by: Joey Jiang <ziyij@ZIYIJ.ap.qualcomm.com>
去掉不需要的景点

Signed-off-by: Joey Jiang <ziyij@ZIYIJ.ap.qualcomm.com>
</commit_message>
<xml_diff>
--- a/sabah.xlsx
+++ b/sabah.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="行程" sheetId="2" r:id="rId1"/>
@@ -331,26 +331,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Dreamy Island Transport 梦之岛快艇DBKK 244530
- Kota Kinabalu, Sabah, Malaysia.
- +6016 803 3503(MR.Ang洪叔),
- +601119070966(Ms.Mun雅雯)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>环滩岛去不成。考虑迪加岛</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>委士顿（</t>
     </r>
     <r>
@@ -378,12 +358,32 @@
   <si>
     <t>海龟岛公园</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dreamy Island Transport 梦之岛快艇DBKK 244530
+ Kota Kinabalu, Sabah, Malaysia.
+ +6016 803 3503(MR.Ang洪叔),
+ +601119070966(Ms.Mun雅雯)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>环滩岛去不成。考虑迪加岛</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,14 +469,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -532,6 +524,31 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -616,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,20 +652,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,27 +671,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1146,14 +1166,14 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
@@ -1162,25 +1182,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1188,246 +1208,246 @@
       <c r="A2" s="21">
         <v>41612</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="22"/>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="22"/>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="23"/>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>0.92361111111111116</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="21">
         <v>41613</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="22"/>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="22"/>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>0.625</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="23"/>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="24">
+      <c r="A10" s="19">
         <v>41614</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="25"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="25"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="24">
+      <c r="A13" s="19">
         <v>41615</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="25"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="25"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="24">
+      <c r="A16" s="19">
         <v>41616</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="25"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="25"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="24">
+      <c r="A19" s="19">
         <v>41617</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15" t="s">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="25"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1462,8 +1482,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1513,26 +1533,26 @@
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" s="25" customFormat="1" ht="75">
+      <c r="A6" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>56</v>
+      <c r="D6" s="26" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1">
-      <c r="A8" s="9" t="s">
-        <v>57</v>
+      <c r="A8" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -1543,13 +1563,13 @@
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
@@ -1557,27 +1577,27 @@
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="20"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="E9" s="24"/>
+    </row>
+    <row r="11" spans="1:5" s="25" customFormat="1">
+      <c r="A11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1625,16 +1645,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="17" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>